<commit_message>
Last code version with the old plasticity setup. Now, I will rewrite the assembly of the residual and use a consistent linearization for the Newton loop. A manual copy of this code status is stored my hard drive, too.
</commit_message>
<xml_diff>
--- a/error_computation/frictionless_sliding_analyt_8/frictionless_convergencestudy.xlsx
+++ b/error_computation/frictionless_sliding_analyt_8/frictionless_convergencestudy.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="38">
   <si>
     <t>Database for example "inp_frictionless_sliding_analyt_8"</t>
   </si>
@@ -120,6 +120,15 @@
   <si>
     <t>here, penalty parameter chosen such that displacement error is the same in the coarsest mesh with Nitsche and then scaled 1/h^2</t>
   </si>
+  <si>
+    <t>unstructured meshing</t>
+  </si>
+  <si>
+    <t>inp_frictionless_sliding_analyt_8_420</t>
+  </si>
+  <si>
+    <t>inp_frictionless_sliding_analyt_8_14766</t>
+  </si>
 </sst>
 </file>
 
@@ -221,7 +230,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -378,11 +386,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="70564864"/>
-        <c:axId val="79512320"/>
+        <c:axId val="92542080"/>
+        <c:axId val="92544384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="70564864"/>
+        <c:axId val="92542080"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -390,12 +398,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79512320"/>
+        <c:crossAx val="92544384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="79512320"/>
+        <c:axId val="92544384"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -404,14 +412,13 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70564864"/>
+        <c:crossAx val="92542080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -443,7 +450,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -600,11 +606,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="80035200"/>
-        <c:axId val="80057472"/>
+        <c:axId val="108472192"/>
+        <c:axId val="108473728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="80035200"/>
+        <c:axId val="108472192"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -612,12 +618,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80057472"/>
+        <c:crossAx val="108473728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="80057472"/>
+        <c:axId val="108473728"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -626,14 +632,13 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80035200"/>
+        <c:crossAx val="108472192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -665,7 +670,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -732,11 +736,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="80089856"/>
-        <c:axId val="80091392"/>
+        <c:axId val="108493824"/>
+        <c:axId val="108507904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="80089856"/>
+        <c:axId val="108493824"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -744,12 +748,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80091392"/>
+        <c:crossAx val="108507904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="80091392"/>
+        <c:axId val="108507904"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -758,14 +762,13 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80089856"/>
+        <c:crossAx val="108493824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -954,11 +957,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="80117120"/>
-        <c:axId val="80135296"/>
+        <c:axId val="108668800"/>
+        <c:axId val="108670336"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="80117120"/>
+        <c:axId val="108668800"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -966,12 +969,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80135296"/>
+        <c:crossAx val="108670336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="80135296"/>
+        <c:axId val="108670336"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -980,7 +983,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80117120"/>
+        <c:crossAx val="108668800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1019,7 +1022,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -1176,11 +1178,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="80169216"/>
-        <c:axId val="80175104"/>
+        <c:axId val="108704512"/>
+        <c:axId val="108706048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="80169216"/>
+        <c:axId val="108704512"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1188,12 +1190,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80175104"/>
+        <c:crossAx val="108706048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="80175104"/>
+        <c:axId val="108706048"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1202,14 +1204,13 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80169216"/>
+        <c:crossAx val="108704512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -1225,9 +1226,7 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="de-DE"/>
   <c:chart>
-    <c:title>
-      <c:layout/>
-    </c:title>
+    <c:title/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -1293,11 +1292,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="80182656"/>
-        <c:axId val="80200832"/>
+        <c:axId val="108608128"/>
+        <c:axId val="108622208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="80182656"/>
+        <c:axId val="108608128"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1305,12 +1304,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80200832"/>
+        <c:crossAx val="108622208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="80200832"/>
+        <c:axId val="108622208"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1319,14 +1318,13 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80182656"/>
+        <c:crossAx val="108608128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -1358,7 +1356,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -1515,11 +1512,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="80222464"/>
-        <c:axId val="80236544"/>
+        <c:axId val="108656128"/>
+        <c:axId val="108657664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="80222464"/>
+        <c:axId val="108656128"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1527,12 +1524,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80236544"/>
+        <c:crossAx val="108657664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="80236544"/>
+        <c:axId val="108657664"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1541,14 +1538,13 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80222464"/>
+        <c:crossAx val="108656128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -1580,7 +1576,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -1737,11 +1732,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="80274560"/>
-        <c:axId val="80276096"/>
+        <c:axId val="108761472"/>
+        <c:axId val="108763008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="80274560"/>
+        <c:axId val="108761472"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1749,12 +1744,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80276096"/>
+        <c:crossAx val="108763008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="80276096"/>
+        <c:axId val="108763008"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1763,14 +1758,13 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80274560"/>
+        <c:crossAx val="108761472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -1802,7 +1796,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -1869,11 +1862,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="73472256"/>
-        <c:axId val="73502720"/>
+        <c:axId val="108786816"/>
+        <c:axId val="108788352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="73472256"/>
+        <c:axId val="108786816"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1881,12 +1874,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73502720"/>
+        <c:crossAx val="108788352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="73502720"/>
+        <c:axId val="108788352"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1895,14 +1888,13 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73472256"/>
+        <c:crossAx val="108786816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -2091,11 +2083,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="73524736"/>
-        <c:axId val="73526272"/>
+        <c:axId val="108838912"/>
+        <c:axId val="108840448"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="73524736"/>
+        <c:axId val="108838912"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2103,12 +2095,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73526272"/>
+        <c:crossAx val="108840448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="73526272"/>
+        <c:axId val="108840448"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2117,7 +2109,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73524736"/>
+        <c:crossAx val="108838912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2156,7 +2148,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -2313,11 +2304,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="73585024"/>
-        <c:axId val="73586560"/>
+        <c:axId val="108927616"/>
+        <c:axId val="108937600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="73585024"/>
+        <c:axId val="108927616"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2325,12 +2316,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73586560"/>
+        <c:crossAx val="108937600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="73586560"/>
+        <c:axId val="108937600"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2339,14 +2330,13 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73585024"/>
+        <c:crossAx val="108927616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -2534,11 +2524,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="79534336"/>
-        <c:axId val="79548416"/>
+        <c:axId val="92937216"/>
+        <c:axId val="101819520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="79534336"/>
+        <c:axId val="92937216"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2546,12 +2536,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79548416"/>
+        <c:crossAx val="101819520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="79548416"/>
+        <c:axId val="101819520"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2560,7 +2550,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79534336"/>
+        <c:crossAx val="92937216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2582,9 +2572,7 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="de-DE"/>
   <c:chart>
-    <c:title>
-      <c:layout/>
-    </c:title>
+    <c:title/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -2650,11 +2638,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="73606656"/>
-        <c:axId val="73608192"/>
+        <c:axId val="108953600"/>
+        <c:axId val="108955136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="73606656"/>
+        <c:axId val="108953600"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2662,12 +2650,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73608192"/>
+        <c:crossAx val="108955136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="73608192"/>
+        <c:axId val="108955136"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2676,14 +2664,13 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73606656"/>
+        <c:crossAx val="108953600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -2715,7 +2702,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -2872,11 +2858,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="73638272"/>
-        <c:axId val="73639808"/>
+        <c:axId val="108977152"/>
+        <c:axId val="109003520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="73638272"/>
+        <c:axId val="108977152"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2884,12 +2870,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73639808"/>
+        <c:crossAx val="109003520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="73639808"/>
+        <c:axId val="109003520"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2898,14 +2884,13 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73638272"/>
+        <c:crossAx val="108977152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -2937,7 +2922,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -3094,11 +3078,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="73665152"/>
-        <c:axId val="73675136"/>
+        <c:axId val="109037440"/>
+        <c:axId val="109038976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="73665152"/>
+        <c:axId val="109037440"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3106,12 +3090,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73675136"/>
+        <c:crossAx val="109038976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="73675136"/>
+        <c:axId val="109038976"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3120,14 +3104,13 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73665152"/>
+        <c:crossAx val="109037440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -3143,9 +3126,7 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="de-DE"/>
   <c:chart>
-    <c:title>
-      <c:layout/>
-    </c:title>
+    <c:title/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -3211,11 +3192,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="73707520"/>
-        <c:axId val="73709056"/>
+        <c:axId val="108878848"/>
+        <c:axId val="108884736"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="73707520"/>
+        <c:axId val="108878848"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3223,12 +3204,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73709056"/>
+        <c:crossAx val="108884736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="73709056"/>
+        <c:axId val="108884736"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3237,14 +3218,13 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73707520"/>
+        <c:crossAx val="108878848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -3276,7 +3256,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -3433,11 +3412,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="73882240"/>
-        <c:axId val="73896320"/>
+        <c:axId val="108902272"/>
+        <c:axId val="108903808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="73882240"/>
+        <c:axId val="108902272"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3445,12 +3424,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73896320"/>
+        <c:crossAx val="108903808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="73896320"/>
+        <c:axId val="108903808"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3459,14 +3438,13 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73882240"/>
+        <c:crossAx val="108902272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -3498,7 +3476,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -3655,11 +3632,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="73921664"/>
-        <c:axId val="73923200"/>
+        <c:axId val="109084672"/>
+        <c:axId val="109086208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="73921664"/>
+        <c:axId val="109084672"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3667,12 +3644,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73923200"/>
+        <c:crossAx val="109086208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="73923200"/>
+        <c:axId val="109086208"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3681,14 +3658,13 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73921664"/>
+        <c:crossAx val="109084672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -3704,9 +3680,7 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="de-DE"/>
   <c:chart>
-    <c:title>
-      <c:layout/>
-    </c:title>
+    <c:title/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -3772,11 +3746,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="73812224"/>
-        <c:axId val="73834496"/>
+        <c:axId val="109118592"/>
+        <c:axId val="109120128"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="73812224"/>
+        <c:axId val="109118592"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3784,12 +3758,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73834496"/>
+        <c:crossAx val="109120128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="73834496"/>
+        <c:axId val="109120128"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3798,14 +3772,13 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73812224"/>
+        <c:crossAx val="109118592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -4087,11 +4060,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="107213952"/>
-        <c:axId val="107203200"/>
+        <c:axId val="109146880"/>
+        <c:axId val="109148800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="107213952"/>
+        <c:axId val="109146880"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -4117,12 +4090,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107203200"/>
+        <c:crossAx val="109148800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="107203200"/>
+        <c:axId val="109148800"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -4149,7 +4122,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107213952"/>
+        <c:crossAx val="109146880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4162,7 +4135,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000018" r="0.70000000000000018" t="0.78740157499999996" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4438,11 +4411,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="103829504"/>
-        <c:axId val="103880576"/>
+        <c:axId val="109192320"/>
+        <c:axId val="109194240"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="103829504"/>
+        <c:axId val="109192320"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -4468,12 +4441,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103880576"/>
+        <c:crossAx val="109194240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="103880576"/>
+        <c:axId val="109194240"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -4500,7 +4473,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103829504"/>
+        <c:crossAx val="109192320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4513,7 +4486,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.70000000000000018" r="0.70000000000000018" t="0.78740157499999996" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.78740157499999996" l="0.7000000000000004" r="0.7000000000000004" t="0.78740157499999996" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4789,11 +4762,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="82055936"/>
-        <c:axId val="82101760"/>
+        <c:axId val="109323776"/>
+        <c:axId val="109325696"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="82055936"/>
+        <c:axId val="109323776"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -4819,12 +4792,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82101760"/>
+        <c:crossAx val="109325696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="82101760"/>
+        <c:axId val="109325696"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -4851,7 +4824,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82055936"/>
+        <c:crossAx val="109323776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4864,7 +4837,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7000000000000004" r="0.7000000000000004" t="0.78740157499999996" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000062" r="0.70000000000000062" t="0.78740157499999996" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4890,7 +4863,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -5047,11 +5019,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="79434880"/>
-        <c:axId val="79436416"/>
+        <c:axId val="108243968"/>
+        <c:axId val="108249856"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="79434880"/>
+        <c:axId val="108243968"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -5059,12 +5031,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79436416"/>
+        <c:crossAx val="108249856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="79436416"/>
+        <c:axId val="108249856"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -5073,14 +5045,13 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79434880"/>
+        <c:crossAx val="108243968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -5112,7 +5083,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -5269,11 +5239,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="79486976"/>
-        <c:axId val="79488512"/>
+        <c:axId val="108345216"/>
+        <c:axId val="108346752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="79486976"/>
+        <c:axId val="108345216"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -5281,12 +5251,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79488512"/>
+        <c:crossAx val="108346752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="79488512"/>
+        <c:axId val="108346752"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -5295,14 +5265,13 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79486976"/>
+        <c:crossAx val="108345216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -5334,7 +5303,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -5401,11 +5369,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="79805824"/>
-        <c:axId val="79819904"/>
+        <c:axId val="108366848"/>
+        <c:axId val="108376832"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="79805824"/>
+        <c:axId val="108366848"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -5413,12 +5381,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79819904"/>
+        <c:crossAx val="108376832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="79819904"/>
+        <c:axId val="108376832"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -5427,14 +5395,13 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79805824"/>
+        <c:crossAx val="108366848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -5466,7 +5433,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -5533,11 +5499,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="79852288"/>
-        <c:axId val="79853824"/>
+        <c:axId val="108401024"/>
+        <c:axId val="108402560"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="79852288"/>
+        <c:axId val="108401024"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -5545,12 +5511,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79853824"/>
+        <c:crossAx val="108402560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="79853824"/>
+        <c:axId val="108402560"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -5559,14 +5525,13 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79852288"/>
+        <c:crossAx val="108401024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -5598,7 +5563,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -5755,11 +5719,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="79870976"/>
-        <c:axId val="79880960"/>
+        <c:axId val="108424192"/>
+        <c:axId val="108442368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="79870976"/>
+        <c:axId val="108424192"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -5767,12 +5731,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79880960"/>
+        <c:crossAx val="108442368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="79880960"/>
+        <c:axId val="108442368"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -5781,14 +5745,13 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79870976"/>
+        <c:crossAx val="108424192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -5820,7 +5783,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -5887,11 +5849,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="79925632"/>
-        <c:axId val="79927168"/>
+        <c:axId val="108540288"/>
+        <c:axId val="108541824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="79925632"/>
+        <c:axId val="108540288"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -5899,12 +5861,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79927168"/>
+        <c:crossAx val="108541824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="79927168"/>
+        <c:axId val="108541824"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -5913,14 +5875,13 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79925632"/>
+        <c:crossAx val="108540288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -5952,7 +5913,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -6109,11 +6069,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="80012032"/>
-        <c:axId val="80013568"/>
+        <c:axId val="108571648"/>
+        <c:axId val="108585728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="80012032"/>
+        <c:axId val="108571648"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -6121,12 +6081,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80013568"/>
+        <c:crossAx val="108585728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="80013568"/>
+        <c:axId val="108585728"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -6135,14 +6095,13 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80012032"/>
+        <c:crossAx val="108571648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -7314,10 +7273,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y166"/>
+  <dimension ref="A1:Y178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A144" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K176" sqref="K176"/>
+    <sheetView tabSelected="1" topLeftCell="A138" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G151" sqref="G151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -10027,7 +9986,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="161" spans="14:16">
+    <row r="161" spans="1:16">
       <c r="O161">
         <v>0.1</v>
       </c>
@@ -10035,12 +9994,12 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="162" spans="14:16">
+    <row r="162" spans="1:16">
       <c r="N162" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="163" spans="14:16">
+    <row r="163" spans="1:16">
       <c r="N163" t="s">
         <v>19</v>
       </c>
@@ -10051,7 +10010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="14:16">
+    <row r="164" spans="1:16">
       <c r="O164">
         <v>0.1</v>
       </c>
@@ -10059,7 +10018,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="165" spans="14:16">
+    <row r="165" spans="1:16">
       <c r="N165" t="s">
         <v>20</v>
       </c>
@@ -10070,12 +10029,63 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="14:16">
+    <row r="166" spans="1:16">
       <c r="O166">
         <v>0.1</v>
       </c>
       <c r="P166">
         <v>1E-4</v>
+      </c>
+    </row>
+    <row r="176" spans="1:16">
+      <c r="A176" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="177" spans="2:9">
+      <c r="B177" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D177">
+        <v>420</v>
+      </c>
+      <c r="E177">
+        <v>484</v>
+      </c>
+      <c r="F177">
+        <v>512</v>
+      </c>
+      <c r="G177">
+        <v>8.5985000000000006E-2</v>
+      </c>
+      <c r="H177">
+        <v>0.28201999999999999</v>
+      </c>
+      <c r="I177">
+        <v>6.8597000000000005E-2</v>
+      </c>
+    </row>
+    <row r="178" spans="2:9">
+      <c r="B178" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D178">
+        <v>14766</v>
+      </c>
+      <c r="E178">
+        <v>15162</v>
+      </c>
+      <c r="F178">
+        <v>15318</v>
+      </c>
+      <c r="G178">
+        <v>1.5759000000000001E-3</v>
+      </c>
+      <c r="H178">
+        <v>0.29108000000000001</v>
+      </c>
+      <c r="I178">
+        <v>0.55823999999999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Penalty works with plasticity. I am not sure about Nitsche. There is some trouble with the second Nitsche term. When the second Nitsche term is neglected, then the displacement field seems to be ok. A more detailed analysis has to be performed.
</commit_message>
<xml_diff>
--- a/error_computation/frictionless_sliding_analyt_8/frictionless_convergencestudy.xlsx
+++ b/error_computation/frictionless_sliding_analyt_8/frictionless_convergencestudy.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="240" windowWidth="6300" windowHeight="4125"/>
+    <workbookView xWindow="480" yWindow="240" windowWidth="6300" windowHeight="4125" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Error norms" sheetId="4" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="48">
   <si>
     <t>Database for example "inp_frictionless_sliding_analyt_8"</t>
   </si>
@@ -119,15 +119,6 @@
     <t>here, penalty parameter chosen such that displacement error is the same in the coarsest mesh with Nitsche and then scaled 1/h^2</t>
   </si>
   <si>
-    <t>unstructured meshing</t>
-  </si>
-  <si>
-    <t>inp_frictionless_sliding_analyt_8_420</t>
-  </si>
-  <si>
-    <t>inp_frictionless_sliding_analyt_8_14766</t>
-  </si>
-  <si>
     <t>choose stabilization parameter automatically</t>
   </si>
   <si>
@@ -147,6 +138,27 @@
   </si>
   <si>
     <t>Traction</t>
+  </si>
+  <si>
+    <t>Parameters</t>
+  </si>
+  <si>
+    <t>mesh size h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">displacement </t>
+  </si>
+  <si>
+    <t>energy</t>
+  </si>
+  <si>
+    <t>traction</t>
+  </si>
+  <si>
+    <t>Lagrange</t>
+  </si>
+  <si>
+    <t>penalty</t>
   </si>
 </sst>
 </file>
@@ -429,11 +441,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="75156864"/>
-        <c:axId val="82732160"/>
+        <c:axId val="67040768"/>
+        <c:axId val="74273920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="75156864"/>
+        <c:axId val="67040768"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -441,12 +453,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82732160"/>
+        <c:crossAx val="74273920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="82732160"/>
+        <c:axId val="74273920"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -455,7 +467,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75156864"/>
+        <c:crossAx val="67040768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -649,11 +661,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="87506944"/>
-        <c:axId val="87508480"/>
+        <c:axId val="79052800"/>
+        <c:axId val="79054336"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87506944"/>
+        <c:axId val="79052800"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -661,12 +673,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87508480"/>
+        <c:crossAx val="79054336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87508480"/>
+        <c:axId val="79054336"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -675,7 +687,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87506944"/>
+        <c:crossAx val="79052800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -780,11 +792,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="87540864"/>
-        <c:axId val="87542400"/>
+        <c:axId val="79082624"/>
+        <c:axId val="79084160"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87540864"/>
+        <c:axId val="79082624"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -792,12 +804,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87542400"/>
+        <c:crossAx val="79084160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87542400"/>
+        <c:axId val="79084160"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -806,7 +818,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87540864"/>
+        <c:crossAx val="79082624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1002,11 +1014,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="87449600"/>
-        <c:axId val="87451136"/>
+        <c:axId val="78999552"/>
+        <c:axId val="79001088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87449600"/>
+        <c:axId val="78999552"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1014,12 +1026,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87451136"/>
+        <c:crossAx val="79001088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87451136"/>
+        <c:axId val="79001088"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1028,7 +1040,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87449600"/>
+        <c:crossAx val="78999552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1223,11 +1235,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="87485056"/>
-        <c:axId val="87568768"/>
+        <c:axId val="79018624"/>
+        <c:axId val="79114624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87485056"/>
+        <c:axId val="79018624"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1235,12 +1247,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87568768"/>
+        <c:crossAx val="79114624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87568768"/>
+        <c:axId val="79114624"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1249,7 +1261,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87485056"/>
+        <c:crossAx val="79018624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1339,11 +1351,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="87589632"/>
-        <c:axId val="87591168"/>
+        <c:axId val="79135488"/>
+        <c:axId val="79137024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87589632"/>
+        <c:axId val="79135488"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1351,12 +1363,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87591168"/>
+        <c:crossAx val="79137024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87591168"/>
+        <c:axId val="79137024"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1365,7 +1377,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87589632"/>
+        <c:crossAx val="79135488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1561,11 +1573,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="87629184"/>
-        <c:axId val="87643264"/>
+        <c:axId val="79175040"/>
+        <c:axId val="79189120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87629184"/>
+        <c:axId val="79175040"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1573,12 +1585,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87643264"/>
+        <c:crossAx val="79189120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87643264"/>
+        <c:axId val="79189120"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1587,7 +1599,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87629184"/>
+        <c:crossAx val="79175040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1782,11 +1794,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="87656704"/>
-        <c:axId val="87674880"/>
+        <c:axId val="79202560"/>
+        <c:axId val="79220736"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87656704"/>
+        <c:axId val="79202560"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1794,12 +1806,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87674880"/>
+        <c:crossAx val="79220736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87674880"/>
+        <c:axId val="79220736"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1808,7 +1820,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87656704"/>
+        <c:crossAx val="79202560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1913,11 +1925,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="87686144"/>
-        <c:axId val="87831296"/>
+        <c:axId val="79232000"/>
+        <c:axId val="79373056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87686144"/>
+        <c:axId val="79232000"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1925,12 +1937,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87831296"/>
+        <c:crossAx val="79373056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87831296"/>
+        <c:axId val="79373056"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1939,7 +1951,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87686144"/>
+        <c:crossAx val="79232000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2135,11 +2147,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="87865216"/>
-        <c:axId val="87866752"/>
+        <c:axId val="79411072"/>
+        <c:axId val="79412608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87865216"/>
+        <c:axId val="79411072"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2147,12 +2159,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87866752"/>
+        <c:crossAx val="79412608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87866752"/>
+        <c:axId val="79412608"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2161,7 +2173,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87865216"/>
+        <c:crossAx val="79411072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2356,11 +2368,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="87896832"/>
-        <c:axId val="87898368"/>
+        <c:axId val="79504128"/>
+        <c:axId val="79505664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87896832"/>
+        <c:axId val="79504128"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2368,12 +2380,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87898368"/>
+        <c:crossAx val="79505664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87898368"/>
+        <c:axId val="79505664"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2382,7 +2394,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87896832"/>
+        <c:crossAx val="79504128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2576,11 +2588,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="82750080"/>
-        <c:axId val="82764160"/>
+        <c:axId val="74291840"/>
+        <c:axId val="74305920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="82750080"/>
+        <c:axId val="74291840"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2588,12 +2600,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82764160"/>
+        <c:crossAx val="74305920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="82764160"/>
+        <c:axId val="74305920"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2602,7 +2614,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82750080"/>
+        <c:crossAx val="74291840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2692,11 +2704,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="87938944"/>
-        <c:axId val="87940480"/>
+        <c:axId val="79550336"/>
+        <c:axId val="79551872"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87938944"/>
+        <c:axId val="79550336"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2704,12 +2716,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87940480"/>
+        <c:crossAx val="79551872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87940480"/>
+        <c:axId val="79551872"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2718,7 +2730,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87938944"/>
+        <c:crossAx val="79550336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2914,11 +2926,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="87987328"/>
-        <c:axId val="87988864"/>
+        <c:axId val="79594624"/>
+        <c:axId val="79596160"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87987328"/>
+        <c:axId val="79594624"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2926,12 +2938,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87988864"/>
+        <c:crossAx val="79596160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87988864"/>
+        <c:axId val="79596160"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2940,7 +2952,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87987328"/>
+        <c:crossAx val="79594624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3135,11 +3147,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="88014208"/>
-        <c:axId val="88089728"/>
+        <c:axId val="79617408"/>
+        <c:axId val="79635584"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="88014208"/>
+        <c:axId val="79617408"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3147,12 +3159,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88089728"/>
+        <c:crossAx val="79635584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="88089728"/>
+        <c:axId val="79635584"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3161,7 +3173,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88014208"/>
+        <c:crossAx val="79617408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3251,11 +3263,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="88118016"/>
-        <c:axId val="88119552"/>
+        <c:axId val="79663872"/>
+        <c:axId val="79665408"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="88118016"/>
+        <c:axId val="79663872"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3263,12 +3275,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88119552"/>
+        <c:crossAx val="79665408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="88119552"/>
+        <c:axId val="79665408"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3277,7 +3289,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88118016"/>
+        <c:crossAx val="79663872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3473,11 +3485,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="88137088"/>
-        <c:axId val="88036480"/>
+        <c:axId val="79682944"/>
+        <c:axId val="79451264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="88137088"/>
+        <c:axId val="79682944"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3485,12 +3497,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88036480"/>
+        <c:crossAx val="79451264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="88036480"/>
+        <c:axId val="79451264"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3499,7 +3511,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88137088"/>
+        <c:crossAx val="79682944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3694,11 +3706,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="88053632"/>
-        <c:axId val="88055168"/>
+        <c:axId val="79468416"/>
+        <c:axId val="79469952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="88053632"/>
+        <c:axId val="79468416"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3706,12 +3718,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88055168"/>
+        <c:crossAx val="79469952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="88055168"/>
+        <c:axId val="79469952"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3720,7 +3732,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88053632"/>
+        <c:crossAx val="79468416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3810,11 +3822,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="88284160"/>
-        <c:axId val="88294144"/>
+        <c:axId val="79830016"/>
+        <c:axId val="79835904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="88284160"/>
+        <c:axId val="79830016"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3822,12 +3834,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88294144"/>
+        <c:crossAx val="79835904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="88294144"/>
+        <c:axId val="79835904"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3836,7 +3848,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88284160"/>
+        <c:crossAx val="79830016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4064,11 +4076,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="88319872"/>
-        <c:axId val="88211456"/>
+        <c:axId val="79869824"/>
+        <c:axId val="79757312"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="88319872"/>
+        <c:axId val="79869824"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -4094,16 +4106,16 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88211456"/>
+        <c:crossAx val="79757312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="88211456"/>
+        <c:axId val="79757312"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
-          <c:max val="1.0000000000000002E-2"/>
+          <c:max val="1.0000000000000004E-2"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
@@ -4127,7 +4139,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88319872"/>
+        <c:crossAx val="79869824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4355,11 +4367,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="88249856"/>
-        <c:axId val="88251776"/>
+        <c:axId val="79795712"/>
+        <c:axId val="79797632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="88249856"/>
+        <c:axId val="79795712"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -4385,12 +4397,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88251776"/>
+        <c:crossAx val="79797632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="88251776"/>
+        <c:axId val="79797632"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -4417,7 +4429,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88249856"/>
+        <c:crossAx val="79795712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4645,11 +4657,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="88360064"/>
-        <c:axId val="88361984"/>
+        <c:axId val="79967360"/>
+        <c:axId val="79969280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="88360064"/>
+        <c:axId val="79967360"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -4675,12 +4687,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88361984"/>
+        <c:crossAx val="79969280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="88361984"/>
+        <c:axId val="79969280"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -4707,7 +4719,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88360064"/>
+        <c:crossAx val="79967360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4746,6 +4758,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -4902,11 +4915,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="82667008"/>
-        <c:axId val="82668544"/>
+        <c:axId val="74208768"/>
+        <c:axId val="74210304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="82667008"/>
+        <c:axId val="74208768"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -4914,12 +4927,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82668544"/>
+        <c:crossAx val="74210304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="82668544"/>
+        <c:axId val="74210304"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -4928,19 +4941,287 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82667008"/>
+        <c:crossAx val="74208768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.78740157499999996" l="0.70000000000000062" r="0.70000000000000062" t="0.78740157499999996" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart30.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="de-DE"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Penalty parameter</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Error norms'!$A$180:$A$185</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.50619999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.27940999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.14055000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.3892000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.0490999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.5299999999999998E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Error norms'!$B$180:$B$185</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>295000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1170000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2620000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4640000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18500000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Nitsche parameter</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Error norms'!$A$180:$A$185</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.50619999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.27940999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.14055000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.3892000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.0490999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.5299999999999998E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Error norms'!$C$180:$C$185</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6833.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20167</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26833</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>53500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Error norms'!$A$187</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Rate 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Error norms'!$B$187:$B$188</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Error norms'!$C$187:$C$188</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Error norms'!$A$189</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Rate 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Error norms'!$B$189:$B$190</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Error norms'!$C$189:$C$190</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>10000000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="103708928"/>
+        <c:axId val="103707392"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="103708928"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:min val="3.0000000000000002E-2"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0.000000" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="103707392"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="103707392"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:min val="1000"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="103708928"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5122,11 +5403,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="82702720"/>
-        <c:axId val="82704256"/>
+        <c:axId val="78774656"/>
+        <c:axId val="78776192"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="82702720"/>
+        <c:axId val="78774656"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -5134,12 +5415,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82704256"/>
+        <c:crossAx val="78776192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="82704256"/>
+        <c:axId val="78776192"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -5148,7 +5429,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82702720"/>
+        <c:crossAx val="78774656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5252,11 +5533,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="87242240"/>
-        <c:axId val="87243776"/>
+        <c:axId val="78792192"/>
+        <c:axId val="78793728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87242240"/>
+        <c:axId val="78792192"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -5264,12 +5545,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87243776"/>
+        <c:crossAx val="78793728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87243776"/>
+        <c:axId val="78793728"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -5278,7 +5559,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87242240"/>
+        <c:crossAx val="78792192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5316,6 +5597,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -5382,11 +5664,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="87288448"/>
-        <c:axId val="87294336"/>
+        <c:axId val="78826112"/>
+        <c:axId val="78840192"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87288448"/>
+        <c:axId val="78826112"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -5394,12 +5676,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87294336"/>
+        <c:crossAx val="78840192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87294336"/>
+        <c:axId val="78840192"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -5408,13 +5690,14 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87288448"/>
+        <c:crossAx val="78826112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -5602,11 +5885,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="87324160"/>
-        <c:axId val="87325696"/>
+        <c:axId val="78870016"/>
+        <c:axId val="78871552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87324160"/>
+        <c:axId val="78870016"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -5614,12 +5897,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87325696"/>
+        <c:crossAx val="78871552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87325696"/>
+        <c:axId val="78871552"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -5628,7 +5911,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87324160"/>
+        <c:crossAx val="78870016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5732,11 +6015,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="87341696"/>
-        <c:axId val="87359872"/>
+        <c:axId val="78887552"/>
+        <c:axId val="78905728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87341696"/>
+        <c:axId val="78887552"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -5744,12 +6027,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87359872"/>
+        <c:crossAx val="78905728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87359872"/>
+        <c:axId val="78905728"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -5758,7 +6041,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87341696"/>
+        <c:crossAx val="78887552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5953,11 +6236,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="87401600"/>
-        <c:axId val="87403136"/>
+        <c:axId val="78943360"/>
+        <c:axId val="78944896"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87401600"/>
+        <c:axId val="78943360"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -5965,12 +6248,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87403136"/>
+        <c:crossAx val="78944896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87403136"/>
+        <c:axId val="78944896"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -5979,7 +6262,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87401600"/>
+        <c:crossAx val="78943360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6870,6 +7153,36 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>569819</xdr:colOff>
+      <xdr:row>177</xdr:row>
+      <xdr:rowOff>10085</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>191060</xdr:colOff>
+      <xdr:row>191</xdr:row>
+      <xdr:rowOff>88526</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="40" name="Diagramm 39"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId30"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7158,10 +7471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y178"/>
+  <dimension ref="A1:Y190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A146" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D175" sqref="D175"/>
+    <sheetView topLeftCell="A165" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B182" sqref="B182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -9617,7 +9930,7 @@
     </row>
     <row r="140" spans="1:25">
       <c r="A140" s="8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B140" s="9"/>
       <c r="C140" s="8"/>
@@ -10025,54 +10338,127 @@
       </c>
     </row>
     <row r="176" spans="1:16">
-      <c r="A176" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="177" spans="2:9">
-      <c r="B177" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D177">
-        <v>420</v>
-      </c>
-      <c r="E177">
-        <v>484</v>
-      </c>
-      <c r="F177">
-        <v>512</v>
-      </c>
-      <c r="G177">
-        <v>8.5985000000000006E-2</v>
-      </c>
-      <c r="H177">
-        <v>0.28201999999999999</v>
-      </c>
-      <c r="I177">
-        <v>6.8597000000000005E-2</v>
-      </c>
-    </row>
-    <row r="178" spans="2:9">
-      <c r="B178" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D178">
-        <v>14766</v>
-      </c>
-      <c r="E178">
-        <v>15162</v>
-      </c>
-      <c r="F178">
-        <v>15318</v>
-      </c>
-      <c r="G178">
-        <v>1.5759000000000001E-3</v>
-      </c>
-      <c r="H178">
-        <v>0.29108000000000001</v>
-      </c>
-      <c r="I178">
-        <v>0.55823999999999996</v>
+      <c r="A176" s="1"/>
+    </row>
+    <row r="178" spans="1:3">
+      <c r="A178" t="s">
+        <v>41</v>
+      </c>
+      <c r="B178"/>
+    </row>
+    <row r="179" spans="1:3">
+      <c r="A179" t="s">
+        <v>42</v>
+      </c>
+      <c r="B179" t="s">
+        <v>47</v>
+      </c>
+      <c r="C179" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3">
+      <c r="A180" s="15">
+        <v>0.50619999999999998</v>
+      </c>
+      <c r="B180" s="3">
+        <v>90000</v>
+      </c>
+      <c r="C180" s="3">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3">
+      <c r="A181" s="15">
+        <v>0.27940999999999999</v>
+      </c>
+      <c r="B181" s="3">
+        <v>295000</v>
+      </c>
+      <c r="C181" s="3">
+        <v>6833.3</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3">
+      <c r="A182" s="15">
+        <v>0.14055000000000001</v>
+      </c>
+      <c r="B182" s="3">
+        <v>1170000</v>
+      </c>
+      <c r="C182" s="3">
+        <v>13500</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3">
+      <c r="A183" s="15">
+        <v>9.3892000000000003E-2</v>
+      </c>
+      <c r="B183" s="3">
+        <v>2620000</v>
+      </c>
+      <c r="C183" s="3">
+        <v>20167</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3">
+      <c r="A184" s="15">
+        <v>7.0490999999999998E-2</v>
+      </c>
+      <c r="B184" s="3">
+        <v>4640000</v>
+      </c>
+      <c r="C184" s="3">
+        <v>26833</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3">
+      <c r="A185" s="15">
+        <v>3.5299999999999998E-2</v>
+      </c>
+      <c r="B185" s="3">
+        <v>18500000</v>
+      </c>
+      <c r="C185" s="3">
+        <v>53500</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3">
+      <c r="A187" t="s">
+        <v>19</v>
+      </c>
+      <c r="B187" s="5">
+        <v>0.03</v>
+      </c>
+      <c r="C187" s="3">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3">
+      <c r="B188" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="C188" s="3">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3">
+      <c r="A189" t="s">
+        <v>20</v>
+      </c>
+      <c r="B189" s="5">
+        <v>0.03</v>
+      </c>
+      <c r="C189" s="3">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3">
+      <c r="B190" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="C190" s="3">
+        <v>100000</v>
       </c>
     </row>
   </sheetData>
@@ -10084,10 +10470,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22:D27"/>
+    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -10102,7 +10488,7 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -10110,567 +10496,727 @@
         <v>18</v>
       </c>
       <c r="G5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="15">
-        <v>0.50619999999999998</v>
-      </c>
-      <c r="B6" s="15">
-        <v>5.2655999999999996E-3</v>
-      </c>
-      <c r="C6" s="15">
-        <v>0.32915</v>
-      </c>
-      <c r="D6" s="15">
-        <v>4.2683</v>
-      </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="15">
-        <v>0.50619999999999998</v>
-      </c>
-      <c r="H6" s="15">
-        <v>5.2655999999999996E-3</v>
-      </c>
-      <c r="I6" s="15">
-        <v>5.2431999999999999E-3</v>
-      </c>
-      <c r="J6" s="15">
-        <v>5.2491999999999999E-3</v>
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" t="s">
+        <v>46</v>
+      </c>
+      <c r="I6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J6" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="15">
-        <v>0.27940999999999999</v>
+        <v>0.50619999999999998</v>
       </c>
       <c r="B7" s="15">
-        <v>1.6842000000000001E-3</v>
+        <v>5.2655999999999996E-3</v>
       </c>
       <c r="C7" s="15">
-        <v>0.18454000000000001</v>
+        <v>0.32915</v>
       </c>
       <c r="D7" s="15">
-        <v>7.4970999999999997</v>
+        <v>4.2683</v>
       </c>
       <c r="E7" s="16"/>
       <c r="F7" s="16"/>
       <c r="G7" s="15">
-        <v>0.27940999999999999</v>
+        <v>0.50619999999999998</v>
       </c>
       <c r="H7" s="15">
-        <v>1.6842000000000001E-3</v>
+        <v>5.2655999999999996E-3</v>
       </c>
       <c r="I7" s="15">
-        <v>1.6561E-3</v>
+        <v>5.2431999999999999E-3</v>
       </c>
       <c r="J7" s="15">
-        <v>1.6666999999999999E-3</v>
+        <v>5.2491999999999999E-3</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="15">
-        <v>0.14055000000000001</v>
+        <v>0.27940999999999999</v>
       </c>
       <c r="B8" s="15">
-        <v>5.0378E-4</v>
+        <v>1.6842000000000001E-3</v>
       </c>
       <c r="C8" s="15">
-        <v>9.2914999999999998E-2</v>
+        <v>0.18454000000000001</v>
       </c>
       <c r="D8" s="15">
-        <v>15.3284</v>
+        <v>7.4970999999999997</v>
       </c>
       <c r="E8" s="16"/>
       <c r="F8" s="16"/>
       <c r="G8" s="15">
-        <v>0.14055000000000001</v>
+        <v>0.27940999999999999</v>
       </c>
       <c r="H8" s="15">
-        <v>5.0378E-4</v>
+        <v>1.6842000000000001E-3</v>
       </c>
       <c r="I8" s="15">
-        <v>4.9487999999999995E-4</v>
+        <v>1.6561E-3</v>
       </c>
       <c r="J8" s="15">
-        <v>5.0233999999999999E-4</v>
+        <v>1.6666999999999999E-3</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="15">
-        <v>9.3892000000000003E-2</v>
+        <v>0.14055000000000001</v>
       </c>
       <c r="B9" s="15">
-        <v>2.5033E-4</v>
+        <v>5.0378E-4</v>
       </c>
       <c r="C9" s="15">
-        <v>6.2086000000000002E-2</v>
+        <v>9.2914999999999998E-2</v>
       </c>
       <c r="D9" s="15">
-        <v>23.099299999999999</v>
+        <v>15.3284</v>
       </c>
       <c r="E9" s="16"/>
       <c r="F9" s="16"/>
       <c r="G9" s="15">
-        <v>9.3892000000000003E-2</v>
+        <v>0.14055000000000001</v>
       </c>
       <c r="H9" s="15">
-        <v>2.5033E-4</v>
+        <v>5.0378E-4</v>
       </c>
       <c r="I9" s="15">
-        <v>2.4644000000000001E-4</v>
+        <v>4.9487999999999995E-4</v>
       </c>
       <c r="J9" s="15">
-        <v>2.5024999999999998E-4</v>
+        <v>5.0233999999999999E-4</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="15">
-        <v>7.0490999999999998E-2</v>
+        <v>9.3892000000000003E-2</v>
       </c>
       <c r="B10" s="15">
-        <v>1.5364999999999999E-4</v>
+        <v>2.5033E-4</v>
       </c>
       <c r="C10" s="15">
-        <v>4.6618E-2</v>
+        <v>6.2086000000000002E-2</v>
       </c>
       <c r="D10" s="15">
-        <v>30.856200000000001</v>
+        <v>23.099299999999999</v>
       </c>
       <c r="E10" s="16"/>
       <c r="F10" s="16"/>
       <c r="G10" s="15">
-        <v>7.0490999999999998E-2</v>
+        <v>9.3892000000000003E-2</v>
       </c>
       <c r="H10" s="15">
-        <v>1.5364999999999999E-4</v>
+        <v>2.5033E-4</v>
       </c>
       <c r="I10" s="15">
-        <v>1.5165E-4</v>
+        <v>2.4644000000000001E-4</v>
       </c>
       <c r="J10" s="15">
-        <v>1.5384E-4</v>
+        <v>2.5024999999999998E-4</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="15">
-        <v>3.5299999999999998E-2</v>
+        <v>7.0490999999999998E-2</v>
       </c>
       <c r="B11" s="15">
-        <v>4.9234000000000003E-5</v>
+        <v>1.5364999999999999E-4</v>
       </c>
       <c r="C11" s="15">
-        <v>2.3348000000000001E-2</v>
+        <v>4.6618E-2</v>
       </c>
       <c r="D11" s="15">
-        <v>61.853999999999999</v>
+        <v>30.856200000000001</v>
       </c>
       <c r="E11" s="16"/>
       <c r="F11" s="16"/>
       <c r="G11" s="15">
+        <v>7.0490999999999998E-2</v>
+      </c>
+      <c r="H11" s="15">
+        <v>1.5364999999999999E-4</v>
+      </c>
+      <c r="I11" s="15">
+        <v>1.5165E-4</v>
+      </c>
+      <c r="J11" s="15">
+        <v>1.5384E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="15">
         <v>3.5299999999999998E-2</v>
       </c>
-      <c r="H11" s="15">
+      <c r="B12" s="15">
         <v>4.9234000000000003E-5</v>
       </c>
-      <c r="I11" s="15">
-        <v>4.8841999999999998E-5</v>
-      </c>
-      <c r="J11" s="15">
-        <v>4.9327999999999999E-5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="16"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
+      <c r="C12" s="15">
+        <v>2.3348000000000001E-2</v>
+      </c>
+      <c r="D12" s="15">
+        <v>61.853999999999999</v>
+      </c>
       <c r="E12" s="16"/>
       <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
+      <c r="G12" s="15">
+        <v>3.5299999999999998E-2</v>
+      </c>
+      <c r="H12" s="15">
+        <v>4.9234000000000003E-5</v>
+      </c>
+      <c r="I12" s="15">
+        <v>4.8841999999999998E-5</v>
+      </c>
+      <c r="J12" s="15">
+        <v>4.9327999999999999E-5</v>
+      </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="16" t="s">
-        <v>39</v>
-      </c>
+      <c r="A13" s="16"/>
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
       <c r="E13" s="16"/>
       <c r="F13" s="16"/>
-      <c r="G13" s="16" t="s">
-        <v>42</v>
-      </c>
+      <c r="G13" s="16"/>
       <c r="H13" s="16"/>
       <c r="I13" s="16"/>
       <c r="J13" s="16"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="15">
-        <v>0.50619999999999998</v>
-      </c>
-      <c r="B14" s="15">
-        <v>5.2431999999999999E-3</v>
-      </c>
-      <c r="C14" s="15">
-        <v>0.32779000000000003</v>
-      </c>
-      <c r="D14" s="15">
-        <v>0.54015999999999997</v>
-      </c>
+      <c r="A14" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
       <c r="E14" s="16"/>
       <c r="F14" s="16"/>
-      <c r="G14" s="15">
-        <v>0.50619999999999998</v>
-      </c>
-      <c r="H14" s="15">
-        <v>0.32915</v>
-      </c>
-      <c r="I14" s="15">
-        <v>0.32779000000000003</v>
-      </c>
-      <c r="J14" s="15">
-        <v>0.32662000000000002</v>
-      </c>
+      <c r="G14" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="15">
-        <v>0.27940999999999999</v>
-      </c>
-      <c r="B15" s="15">
-        <v>1.6561E-3</v>
-      </c>
-      <c r="C15" s="15">
-        <v>0.18404999999999999</v>
-      </c>
-      <c r="D15" s="15">
-        <v>0.35819000000000001</v>
-      </c>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="15">
-        <v>0.27940999999999999</v>
-      </c>
-      <c r="H15" s="15">
-        <v>0.18454000000000001</v>
-      </c>
-      <c r="I15" s="15">
-        <v>0.18404999999999999</v>
-      </c>
-      <c r="J15" s="15">
-        <v>0.18382999999999999</v>
+      <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" t="s">
+        <v>45</v>
+      </c>
+      <c r="G15" t="s">
+        <v>42</v>
+      </c>
+      <c r="H15" t="s">
+        <v>46</v>
+      </c>
+      <c r="I15" t="s">
+        <v>36</v>
+      </c>
+      <c r="J15" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="15">
-        <v>0.14055000000000001</v>
+        <v>0.50619999999999998</v>
       </c>
       <c r="B16" s="15">
-        <v>4.9487999999999995E-4</v>
+        <v>5.2431999999999999E-3</v>
       </c>
       <c r="C16" s="15">
-        <v>9.2779E-2</v>
+        <v>0.32779000000000003</v>
       </c>
       <c r="D16" s="15">
-        <v>0.21196000000000001</v>
+        <v>0.54015999999999997</v>
       </c>
       <c r="E16" s="16"/>
       <c r="F16" s="16"/>
       <c r="G16" s="15">
-        <v>0.14055000000000001</v>
+        <v>0.50619999999999998</v>
       </c>
       <c r="H16" s="15">
-        <v>9.2914999999999998E-2</v>
+        <v>0.32915</v>
       </c>
       <c r="I16" s="15">
-        <v>9.2779E-2</v>
+        <v>0.32779000000000003</v>
       </c>
       <c r="J16" s="15">
-        <v>9.2743999999999993E-2</v>
+        <v>0.32662000000000002</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="15">
-        <v>9.3892000000000003E-2</v>
+        <v>0.27940999999999999</v>
       </c>
       <c r="B17" s="15">
-        <v>2.4644000000000001E-4</v>
+        <v>1.6561E-3</v>
       </c>
       <c r="C17" s="15">
-        <v>6.2023000000000002E-2</v>
+        <v>0.18404999999999999</v>
       </c>
       <c r="D17" s="15">
-        <v>0.15285000000000001</v>
+        <v>0.35819000000000001</v>
       </c>
       <c r="E17" s="16"/>
       <c r="F17" s="16"/>
       <c r="G17" s="15">
-        <v>9.3892000000000003E-2</v>
+        <v>0.27940999999999999</v>
       </c>
       <c r="H17" s="15">
-        <v>6.2086000000000002E-2</v>
+        <v>0.18454000000000001</v>
       </c>
       <c r="I17" s="15">
-        <v>6.2023000000000002E-2</v>
+        <v>0.18404999999999999</v>
       </c>
       <c r="J17" s="15">
-        <v>6.2011999999999998E-2</v>
+        <v>0.18382999999999999</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="15">
-        <v>7.0490999999999998E-2</v>
+        <v>0.14055000000000001</v>
       </c>
       <c r="B18" s="15">
-        <v>1.5165E-4</v>
+        <v>4.9487999999999995E-4</v>
       </c>
       <c r="C18" s="15">
-        <v>4.6581999999999998E-2</v>
+        <v>9.2779E-2</v>
       </c>
       <c r="D18" s="15">
-        <v>0.12267</v>
+        <v>0.21196000000000001</v>
       </c>
       <c r="E18" s="16"/>
       <c r="F18" s="16"/>
       <c r="G18" s="15">
-        <v>7.0490999999999998E-2</v>
+        <v>0.14055000000000001</v>
       </c>
       <c r="H18" s="15">
-        <v>4.6618E-2</v>
+        <v>9.2914999999999998E-2</v>
       </c>
       <c r="I18" s="15">
-        <v>4.6581999999999998E-2</v>
+        <v>9.2779E-2</v>
       </c>
       <c r="J18" s="15">
-        <v>4.6575999999999999E-2</v>
+        <v>9.2743999999999993E-2</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="15">
-        <v>3.5299999999999998E-2</v>
+        <v>9.3892000000000003E-2</v>
       </c>
       <c r="B19" s="15">
-        <v>4.8841999999999998E-5</v>
+        <v>2.4644000000000001E-4</v>
       </c>
       <c r="C19" s="15">
-        <v>2.3338000000000001E-2</v>
+        <v>6.2023000000000002E-2</v>
       </c>
       <c r="D19" s="15">
-        <v>7.2650000000000006E-2</v>
+        <v>0.15285000000000001</v>
       </c>
       <c r="E19" s="16"/>
       <c r="F19" s="16"/>
       <c r="G19" s="15">
-        <v>3.5299999999999998E-2</v>
+        <v>9.3892000000000003E-2</v>
       </c>
       <c r="H19" s="15">
-        <v>2.3348000000000001E-2</v>
+        <v>6.2086000000000002E-2</v>
       </c>
       <c r="I19" s="15">
-        <v>2.3338000000000001E-2</v>
+        <v>6.2023000000000002E-2</v>
       </c>
       <c r="J19" s="15">
-        <v>2.3338000000000001E-2</v>
+        <v>6.2011999999999998E-2</v>
       </c>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="16"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
+      <c r="A20" s="15">
+        <v>7.0490999999999998E-2</v>
+      </c>
+      <c r="B20" s="15">
+        <v>1.5165E-4</v>
+      </c>
+      <c r="C20" s="15">
+        <v>4.6581999999999998E-2</v>
+      </c>
+      <c r="D20" s="15">
+        <v>0.12267</v>
+      </c>
       <c r="E20" s="16"/>
       <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="16"/>
+      <c r="G20" s="15">
+        <v>7.0490999999999998E-2</v>
+      </c>
+      <c r="H20" s="15">
+        <v>4.6618E-2</v>
+      </c>
+      <c r="I20" s="15">
+        <v>4.6581999999999998E-2</v>
+      </c>
+      <c r="J20" s="15">
+        <v>4.6575999999999999E-2</v>
+      </c>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
+      <c r="A21" s="15">
+        <v>3.5299999999999998E-2</v>
+      </c>
+      <c r="B21" s="15">
+        <v>4.8841999999999998E-5</v>
+      </c>
+      <c r="C21" s="15">
+        <v>2.3338000000000001E-2</v>
+      </c>
+      <c r="D21" s="15">
+        <v>7.2650000000000006E-2</v>
+      </c>
       <c r="E21" s="16"/>
       <c r="F21" s="16"/>
-      <c r="G21" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
+      <c r="G21" s="15">
+        <v>3.5299999999999998E-2</v>
+      </c>
+      <c r="H21" s="15">
+        <v>2.3348000000000001E-2</v>
+      </c>
+      <c r="I21" s="15">
+        <v>2.3338000000000001E-2</v>
+      </c>
+      <c r="J21" s="15">
+        <v>2.3338000000000001E-2</v>
+      </c>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="15">
-        <v>0.50619999999999998</v>
-      </c>
-      <c r="B22" s="15">
-        <v>5.2491999999999999E-3</v>
-      </c>
-      <c r="C22" s="15">
-        <v>0.32662000000000002</v>
-      </c>
-      <c r="D22" s="15">
-        <v>0.20412</v>
-      </c>
+      <c r="A22" s="16"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
       <c r="E22" s="16"/>
       <c r="F22" s="16"/>
-      <c r="G22" s="15">
-        <v>0.50619999999999998</v>
-      </c>
-      <c r="H22" s="15">
-        <v>4.2683</v>
-      </c>
-      <c r="I22" s="15">
-        <v>0.54015999999999997</v>
-      </c>
-      <c r="J22" s="15">
-        <v>0.20412</v>
-      </c>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="15">
-        <v>0.27940999999999999</v>
-      </c>
-      <c r="B23" s="15">
-        <v>1.6666999999999999E-3</v>
-      </c>
-      <c r="C23" s="15">
-        <v>0.18382999999999999</v>
-      </c>
-      <c r="D23" s="15">
-        <v>0.11226999999999999</v>
-      </c>
+      <c r="A23" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
       <c r="E23" s="16"/>
       <c r="F23" s="16"/>
-      <c r="G23" s="15">
-        <v>0.27940999999999999</v>
-      </c>
-      <c r="H23" s="15">
-        <v>7.4970999999999997</v>
-      </c>
-      <c r="I23" s="15">
-        <v>0.35819000000000001</v>
-      </c>
-      <c r="J23" s="15">
-        <v>0.11226999999999999</v>
-      </c>
+      <c r="G23" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="15">
-        <v>0.14055000000000001</v>
-      </c>
-      <c r="B24" s="15">
-        <v>5.0233999999999999E-4</v>
-      </c>
-      <c r="C24" s="15">
-        <v>9.2743999999999993E-2</v>
-      </c>
-      <c r="D24" s="15">
-        <v>5.3135000000000002E-2</v>
-      </c>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="15">
-        <v>0.14055000000000001</v>
-      </c>
-      <c r="H24" s="15">
-        <v>15.3284</v>
-      </c>
-      <c r="I24" s="15">
-        <v>0.21196000000000001</v>
-      </c>
-      <c r="J24" s="15">
-        <v>5.3135000000000002E-2</v>
+      <c r="A24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" t="s">
+        <v>45</v>
+      </c>
+      <c r="G24" t="s">
+        <v>42</v>
+      </c>
+      <c r="H24" t="s">
+        <v>46</v>
+      </c>
+      <c r="I24" t="s">
+        <v>36</v>
+      </c>
+      <c r="J24" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="15">
-        <v>9.3892000000000003E-2</v>
+        <v>0.50619999999999998</v>
       </c>
       <c r="B25" s="15">
-        <v>2.5024999999999998E-4</v>
+        <v>5.2491999999999999E-3</v>
       </c>
       <c r="C25" s="15">
-        <v>6.2011999999999998E-2</v>
+        <v>0.32662000000000002</v>
       </c>
       <c r="D25" s="15">
-        <v>3.474E-2</v>
+        <v>0.20412</v>
       </c>
       <c r="E25" s="16"/>
       <c r="F25" s="16"/>
       <c r="G25" s="15">
-        <v>9.3892000000000003E-2</v>
+        <v>0.50619999999999998</v>
       </c>
       <c r="H25" s="15">
-        <v>23.099299999999999</v>
+        <v>4.2683</v>
       </c>
       <c r="I25" s="15">
-        <v>0.15285000000000001</v>
+        <v>0.54015999999999997</v>
       </c>
       <c r="J25" s="15">
-        <v>3.474E-2</v>
+        <v>0.20412</v>
       </c>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="15">
-        <v>7.0490999999999998E-2</v>
+        <v>0.27940999999999999</v>
       </c>
       <c r="B26" s="15">
-        <v>1.5384E-4</v>
+        <v>1.6666999999999999E-3</v>
       </c>
       <c r="C26" s="15">
-        <v>4.6575999999999999E-2</v>
+        <v>0.18382999999999999</v>
       </c>
       <c r="D26" s="15">
-        <v>2.5794999999999998E-2</v>
+        <v>0.11226999999999999</v>
       </c>
       <c r="E26" s="16"/>
       <c r="F26" s="16"/>
       <c r="G26" s="15">
-        <v>7.0490999999999998E-2</v>
+        <v>0.27940999999999999</v>
       </c>
       <c r="H26" s="15">
-        <v>30.856200000000001</v>
+        <v>7.4970999999999997</v>
       </c>
       <c r="I26" s="15">
-        <v>0.12267</v>
+        <v>0.35819000000000001</v>
       </c>
       <c r="J26" s="15">
-        <v>2.5794999999999998E-2</v>
+        <v>0.11226999999999999</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="15">
-        <v>3.5299999999999998E-2</v>
+        <v>0.14055000000000001</v>
       </c>
       <c r="B27" s="15">
-        <v>4.9327999999999999E-5</v>
+        <v>5.0233999999999999E-4</v>
       </c>
       <c r="C27" s="15">
-        <v>2.3338000000000001E-2</v>
+        <v>9.2743999999999993E-2</v>
       </c>
       <c r="D27" s="15">
-        <v>1.2701E-2</v>
+        <v>5.3135000000000002E-2</v>
       </c>
       <c r="E27" s="16"/>
       <c r="F27" s="16"/>
       <c r="G27" s="15">
+        <v>0.14055000000000001</v>
+      </c>
+      <c r="H27" s="15">
+        <v>15.3284</v>
+      </c>
+      <c r="I27" s="15">
+        <v>0.21196000000000001</v>
+      </c>
+      <c r="J27" s="15">
+        <v>5.3135000000000002E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="15">
+        <v>9.3892000000000003E-2</v>
+      </c>
+      <c r="B28" s="15">
+        <v>2.5024999999999998E-4</v>
+      </c>
+      <c r="C28" s="15">
+        <v>6.2011999999999998E-2</v>
+      </c>
+      <c r="D28" s="15">
+        <v>3.474E-2</v>
+      </c>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="15">
+        <v>9.3892000000000003E-2</v>
+      </c>
+      <c r="H28" s="15">
+        <v>23.099299999999999</v>
+      </c>
+      <c r="I28" s="15">
+        <v>0.15285000000000001</v>
+      </c>
+      <c r="J28" s="15">
+        <v>3.474E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="15">
+        <v>7.0490999999999998E-2</v>
+      </c>
+      <c r="B29" s="15">
+        <v>1.5384E-4</v>
+      </c>
+      <c r="C29" s="15">
+        <v>4.6575999999999999E-2</v>
+      </c>
+      <c r="D29" s="15">
+        <v>2.5794999999999998E-2</v>
+      </c>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="15">
+        <v>7.0490999999999998E-2</v>
+      </c>
+      <c r="H29" s="15">
+        <v>30.856200000000001</v>
+      </c>
+      <c r="I29" s="15">
+        <v>0.12267</v>
+      </c>
+      <c r="J29" s="15">
+        <v>2.5794999999999998E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="15">
         <v>3.5299999999999998E-2</v>
       </c>
-      <c r="H27" s="15">
+      <c r="B30" s="15">
+        <v>4.9327999999999999E-5</v>
+      </c>
+      <c r="C30" s="15">
+        <v>2.3338000000000001E-2</v>
+      </c>
+      <c r="D30" s="15">
+        <v>1.2701E-2</v>
+      </c>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="15">
+        <v>3.5299999999999998E-2</v>
+      </c>
+      <c r="H30" s="15">
         <v>61.853999999999999</v>
       </c>
-      <c r="I27" s="15">
+      <c r="I30" s="15">
         <v>7.2650000000000006E-2</v>
       </c>
-      <c r="J27" s="15">
+      <c r="J30" s="15">
         <v>1.2701E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C34" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="15">
+        <v>0.50619999999999998</v>
+      </c>
+      <c r="B35" s="3">
+        <v>90000</v>
+      </c>
+      <c r="C35" s="3">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="15">
+        <v>0.27940999999999999</v>
+      </c>
+      <c r="B36" s="3">
+        <v>295000</v>
+      </c>
+      <c r="C36" s="3">
+        <v>6833.3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="15">
+        <v>0.14055000000000001</v>
+      </c>
+      <c r="B37" s="3">
+        <v>1170000</v>
+      </c>
+      <c r="C37" s="3">
+        <v>13500</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="15">
+        <v>9.3892000000000003E-2</v>
+      </c>
+      <c r="B38" s="3">
+        <v>2620000</v>
+      </c>
+      <c r="C38" s="3">
+        <v>20167</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="15">
+        <v>7.0490999999999998E-2</v>
+      </c>
+      <c r="B39" s="3">
+        <v>4640000</v>
+      </c>
+      <c r="C39" s="3">
+        <v>26833</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="15">
+        <v>3.5299999999999998E-2</v>
+      </c>
+      <c r="B40" s="3">
+        <v>18500000</v>
+      </c>
+      <c r="C40" s="3">
+        <v>53500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>